<commit_message>
Adding times for election odds and update readme
</commit_message>
<xml_diff>
--- a/Election Odds Raw.xlsx
+++ b/Election Odds Raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Developer/2020-Election-Odds-Tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8961AF3B-1F24-A04E-A110-E24F72C04E4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E4F789-4B40-D54D-BD16-A99F042664A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E91F47DA-0CB0-014E-85A8-F4E87909AA65}"/>
+    <workbookView xWindow="-29400" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E91F47DA-0CB0-014E-85A8-F4E87909AA65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="C251" sqref="C251"/>
+      <selection activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>44138</v>
+        <v>44138.416666666664</v>
       </c>
       <c r="B211">
         <v>140</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>44138</v>
+        <v>44138.5</v>
       </c>
       <c r="B212">
         <v>160</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>44138</v>
+        <v>44138.552083333336</v>
       </c>
       <c r="B213">
         <v>170</v>
@@ -3389,7 +3389,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
-        <v>44138</v>
+        <v>44138.583333333336</v>
       </c>
       <c r="B214">
         <v>180</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
-        <v>44138</v>
+        <v>44138.604166666664</v>
       </c>
       <c r="B215">
         <v>175</v>
@@ -3417,7 +3417,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>44138</v>
+        <v>44138.65625</v>
       </c>
       <c r="B216">
         <v>170</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
-        <v>44138</v>
+        <v>44138.75</v>
       </c>
       <c r="B217">
         <v>170</v>
@@ -3445,7 +3445,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
-        <v>44138</v>
+        <v>44138.791666666664</v>
       </c>
       <c r="B218">
         <v>170</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
-        <v>44138</v>
+        <v>44138.798611111109</v>
       </c>
       <c r="B219">
         <v>175</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
-        <v>44138</v>
+        <v>44138.805555555555</v>
       </c>
       <c r="B220">
         <v>190</v>
@@ -3487,7 +3487,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
-        <v>44138</v>
+        <v>44138.809027777781</v>
       </c>
       <c r="B221">
         <v>180</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
-        <v>44138</v>
+        <v>44138.8125</v>
       </c>
       <c r="B222">
         <v>160</v>
@@ -3515,7 +3515,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
-        <v>44138</v>
+        <v>44138.815972222219</v>
       </c>
       <c r="B223">
         <v>145</v>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
-        <v>44138</v>
+        <v>44138.822916666664</v>
       </c>
       <c r="B224">
         <v>125</v>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
-        <v>44138</v>
+        <v>44138.826388888891</v>
       </c>
       <c r="B225">
         <v>105</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
-        <v>44138</v>
+        <v>44138.833333333336</v>
       </c>
       <c r="B226">
         <v>100</v>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
-        <v>44138</v>
+        <v>44138.84375</v>
       </c>
       <c r="B227">
         <v>-110</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
-        <v>44138</v>
+        <v>44138.850694444445</v>
       </c>
       <c r="B228">
         <v>100</v>
@@ -3599,7 +3599,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
-        <v>44138</v>
+        <v>44138.857638888891</v>
       </c>
       <c r="B229">
         <v>120</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
-        <v>44138</v>
+        <v>44138.864583333336</v>
       </c>
       <c r="B230">
         <v>135</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
-        <v>44138</v>
+        <v>44138.868055555555</v>
       </c>
       <c r="B231">
         <v>115</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
-        <v>44138</v>
+        <v>44138.875</v>
       </c>
       <c r="B232">
         <v>110</v>
@@ -3655,7 +3655,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
-        <v>44138</v>
+        <v>44138.888888888891</v>
       </c>
       <c r="B233">
         <v>-110</v>
@@ -3669,7 +3669,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
-        <v>44138</v>
+        <v>44138.892361111109</v>
       </c>
       <c r="B234">
         <v>-120</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
-        <v>44138</v>
+        <v>44138.895833333336</v>
       </c>
       <c r="B235">
         <v>-200</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
-        <v>44138</v>
+        <v>44138.899305555555</v>
       </c>
       <c r="B236">
         <v>-245</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
-        <v>44138</v>
+        <v>44138.902777777781</v>
       </c>
       <c r="B237">
         <v>-220</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
-        <v>44138</v>
+        <v>44138.916666666664</v>
       </c>
       <c r="B238">
         <v>-370</v>
@@ -3739,7 +3739,7 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
-        <v>44138</v>
+        <v>44138.923611111109</v>
       </c>
       <c r="B239">
         <v>-775</v>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
-        <v>44138</v>
+        <v>44138.930555555555</v>
       </c>
       <c r="B240">
         <v>-300</v>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
-        <v>44138</v>
+        <v>44138.940972222219</v>
       </c>
       <c r="B241">
         <v>-250</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
-        <v>44138</v>
+        <v>44138.947916666664</v>
       </c>
       <c r="B242">
         <v>-270</v>
@@ -3795,7 +3795,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
-        <v>44138</v>
+        <v>44138.958333333336</v>
       </c>
       <c r="B243">
         <v>-240</v>
@@ -3809,7 +3809,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
-        <v>44138</v>
+        <v>44138.961805555555</v>
       </c>
       <c r="B244">
         <v>-330</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
-        <v>44138</v>
+        <v>44138.96875</v>
       </c>
       <c r="B245">
         <v>-295</v>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
-        <v>44138</v>
+        <v>44138.979166666664</v>
       </c>
       <c r="B246">
         <v>-190</v>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
-        <v>44138</v>
+        <v>44138.986111111109</v>
       </c>
       <c r="B247">
         <v>-165</v>
@@ -3865,7 +3865,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
-        <v>44138</v>
+        <v>44138.993055555555</v>
       </c>
       <c r="B248">
         <v>-150</v>
@@ -3893,7 +3893,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
-        <v>44139</v>
+        <v>44139.006944444445</v>
       </c>
       <c r="B250">
         <v>-180</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
-        <v>44139</v>
+        <v>44139.010416666664</v>
       </c>
       <c r="B251">
         <v>-150</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
-        <v>44139</v>
+        <v>44139.020833333336</v>
       </c>
       <c r="B252">
         <v>-165</v>
@@ -3935,7 +3935,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
-        <v>44139</v>
+        <v>44139.034722222219</v>
       </c>
       <c r="B253">
         <v>-160</v>
@@ -3949,7 +3949,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
-        <v>44139</v>
+        <v>44139.041666666664</v>
       </c>
       <c r="B254">
         <v>-145</v>
@@ -3963,7 +3963,7 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
-        <v>44139</v>
+        <v>44139.048611111109</v>
       </c>
       <c r="B255">
         <v>-160</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
-        <v>44139</v>
+        <v>44139.375</v>
       </c>
       <c r="B256">
         <v>235</v>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
-        <v>44139</v>
+        <v>44139.416666666664</v>
       </c>
       <c r="B257">
         <v>340</v>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
-        <v>44139</v>
+        <v>44139.458333333336</v>
       </c>
       <c r="B258">
         <v>320</v>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
-        <v>44139</v>
+        <v>44139.510416666664</v>
       </c>
       <c r="B259">
         <v>330</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
-        <v>44139</v>
+        <v>44139.5625</v>
       </c>
       <c r="B260">
         <v>250</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
-        <v>44139</v>
+        <v>44139.565972222219</v>
       </c>
       <c r="B261">
         <v>248</v>
@@ -4061,7 +4061,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
-        <v>44139</v>
+        <v>44139.638888888891</v>
       </c>
       <c r="B262">
         <v>302</v>
@@ -4075,7 +4075,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
-        <v>44139</v>
+        <v>44139.708333333336</v>
       </c>
       <c r="B263">
         <v>490</v>
@@ -4089,7 +4089,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
-        <v>44139</v>
+        <v>44140.017361111109</v>
       </c>
       <c r="B264">
         <v>528</v>
@@ -4103,7 +4103,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
-        <v>44140</v>
+        <v>44140.430555555555</v>
       </c>
       <c r="B265">
         <v>476</v>
@@ -4117,7 +4117,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
-        <v>44140</v>
+        <v>44140.652777777781</v>
       </c>
       <c r="B266">
         <v>675</v>
@@ -4131,7 +4131,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
-        <v>44141</v>
+        <v>44141.388888888891</v>
       </c>
       <c r="B267">
         <v>1050</v>

</xml_diff>

<commit_message>
minor refactoring and add to .gitignore
</commit_message>
<xml_diff>
--- a/Election Odds Raw.xlsx
+++ b/Election Odds Raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Developer/2020-Election-Odds-Tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E4F789-4B40-D54D-BD16-A99F042664A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940C824A-5F7A-FF49-84B2-D2BD74164D2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29400" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E91F47DA-0CB0-014E-85A8-F4E87909AA65}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <t>biden_odds</t>
   </si>
   <si>
-    <t>source</t>
+    <t>odds_source</t>
   </si>
 </sst>
 </file>
@@ -399,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E09FD95-8348-4048-A5D2-30A6965E257B}">
   <dimension ref="A1:D267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="A257" sqref="A257"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>